<commit_message>
revert version can be deleted
</commit_message>
<xml_diff>
--- a/reference/UIdesign.xlsx
+++ b/reference/UIdesign.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="140" windowWidth="25600" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="2060" yWindow="0" windowWidth="26880" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表2" sheetId="2" r:id="rId1"/>
+    <sheet name="开启密码" sheetId="3" r:id="rId2"/>
+    <sheet name="修改密码" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
   <si>
     <t>图片</t>
   </si>
@@ -194,6 +196,224 @@
   </si>
   <si>
     <t>如果有键盘 那么键盘消失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转到p6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码输入错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入正确直接返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开启密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2次密码一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2次密码不一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑色的匡（密码设置成功）出现一下后  自动返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转p7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回p6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见开启密码工作表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑色的匡（输入不一致 请重新输入）出现一下后  自动跳转到‘请输入新密码’界面
+黑色的匡UI可以改变的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码正确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次输入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2次输入一样 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2次输入不一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑色的匡显示后 自动跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑色的匡显示后自动返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入错误 就一直在这个界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码输入正确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见修改密码工作表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果开启密码状态是off的，那么点击这个没有任何效果（没任何反映，不做任何跳转)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置字体 
+p4里的content的字体大小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左上角的返回都一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改字体 并保存返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>勾表示当前字体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">菜单界面
+右滑可以返回（返回p2）
+像微信右滑返回一样
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>除了p4 其他界面右滑都可以返回</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转p9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">保存版本
+保存当前所有记事本的内容到本地
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这时一个输入框
+让用户输入保存版本的标题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参考p10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有任何操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示当前时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存版本后返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果标题是空的，那么active标题的输入框，要求用户输入标题（不保存 不返回)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>键盘下去</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击这个界面深灰色的地方，键盘下去</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为了能点击保存按钮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -201,7 +421,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -244,6 +464,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,7 +490,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,8 +500,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -293,17 +523,34 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1120,6 +1367,2322 @@
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2628900</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直线箭头连接符 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="11214100"/>
+          <a:ext cx="4076700" cy="1346200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3302000</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="203200" y="24510999"/>
+          <a:ext cx="3098800" cy="4648201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>139701</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3128434</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="139701" y="29476700"/>
+          <a:ext cx="2988733" cy="4483100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直线箭头连接符 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="533400" y="24523700"/>
+          <a:ext cx="6146800" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2527300</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直线箭头连接符 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2527300" y="24917400"/>
+          <a:ext cx="4089400" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2349500</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直线箭头连接符 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2349500" y="25298400"/>
+          <a:ext cx="4356100" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直线箭头连接符 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2133600" y="25679400"/>
+          <a:ext cx="4610100" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2374900</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直线箭头连接符 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2374900" y="26035000"/>
+          <a:ext cx="4305300" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2298700</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直线箭头连接符 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2298700" y="26441400"/>
+          <a:ext cx="4406900" cy="558800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直线箭头连接符 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="469900" y="29311600"/>
+          <a:ext cx="6210300" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2717800</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>317500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="直线箭头连接符 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2717800" y="29679900"/>
+          <a:ext cx="3949700" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1879600</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>546100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>800100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="直线箭头连接符 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1879600" y="30505400"/>
+          <a:ext cx="4787900" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1816100</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直线箭头连接符 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1816100" y="31127700"/>
+          <a:ext cx="4826000" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292101</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3255435</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="图片 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="292101" y="34264600"/>
+          <a:ext cx="2963334" cy="4445000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2311400</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直线箭头连接符 51"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2311400" y="35001200"/>
+          <a:ext cx="4406900" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2298700</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="直线箭头连接符 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2298700" y="35369500"/>
+          <a:ext cx="4381500" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="直线箭头连接符 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2438400" y="35763200"/>
+          <a:ext cx="4254500" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3276601</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="图片 58"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152401" y="39001700"/>
+          <a:ext cx="3124200" cy="4686300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1739900</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="直线箭头连接符 60"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1739900" y="39395400"/>
+          <a:ext cx="4940300" cy="965200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="直线箭头连接符 62"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1752600" y="40525700"/>
+          <a:ext cx="4965700" cy="673100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2476500</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="直线箭头连接符 64"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2476500" y="41478200"/>
+          <a:ext cx="4191000" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3302000</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="图片 65"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="177800" y="43967400"/>
+          <a:ext cx="3124200" cy="4686300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="直线箭头连接符 71"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="749300" y="46202600"/>
+          <a:ext cx="5905500" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>279401</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>177801</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1536701" y="444500"/>
+          <a:ext cx="1549400" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>359834</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1447801" y="3111500"/>
+          <a:ext cx="1820333" cy="2730500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330199</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5562600" y="3136901"/>
+          <a:ext cx="1803399" cy="2705099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>486833</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5651500" y="6985000"/>
+          <a:ext cx="1871133" cy="2806700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9194800" y="3130550"/>
+          <a:ext cx="1790700" cy="2686050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63502</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="406400"/>
+          <a:ext cx="1549401" cy="2324102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直线箭头连接符 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2565400" y="1587500"/>
+          <a:ext cx="4064000" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直线箭头连接符 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2540000" y="2133600"/>
+          <a:ext cx="6705600" cy="63500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直线箭头连接符 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2324100" y="4483100"/>
+          <a:ext cx="3848100" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直线箭头连接符 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6845300" y="4483100"/>
+          <a:ext cx="2705100" cy="25400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直线箭头连接符 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6464300" y="5041900"/>
+          <a:ext cx="12700" cy="2806700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="肘形连接符 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="2343150" y="5124450"/>
+          <a:ext cx="4013200" cy="3644900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 633"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直线箭头连接符 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10312400" y="5029200"/>
+          <a:ext cx="2044700" cy="165100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>469901</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>313268</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3149601" y="241300"/>
+          <a:ext cx="2319867" cy="3479800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>88899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>165098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3124200" y="4660899"/>
+          <a:ext cx="2463800" cy="3695699"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>660399</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6997700" y="323853"/>
+          <a:ext cx="2120899" cy="3181347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>681567</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10604500" y="596900"/>
+          <a:ext cx="1837267" cy="2755900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10591800" y="4324350"/>
+          <a:ext cx="1892300" cy="2838450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>512233</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14605000" y="571500"/>
+          <a:ext cx="1794933" cy="2692400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直线箭头连接符 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="774700" y="1943100"/>
+          <a:ext cx="3098800" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="直线箭头连接符 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3937000" y="2705100"/>
+          <a:ext cx="63500" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直线箭头连接符 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4648200" y="1981200"/>
+          <a:ext cx="3200400" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直线箭头连接符 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8305800" y="1943100"/>
+          <a:ext cx="2984500" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直线箭头连接符 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11772900" y="2006600"/>
+          <a:ext cx="3162300" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直线箭头连接符 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11226800" y="2603500"/>
+          <a:ext cx="50800" cy="2806700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="肘形连接符 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="4572000" y="2717800"/>
+          <a:ext cx="6692900" cy="3670300"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 70114"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直线箭头连接符 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14732000" y="2489200"/>
+          <a:ext cx="304800" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="右弧形箭头 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2171700" y="6426200"/>
+          <a:ext cx="1346200" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedRightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="肘形连接符 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3689350" y="3054350"/>
+          <a:ext cx="5168900" cy="4292600"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -369"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -1467,11 +4030,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G225" sqref="G225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1859,6 +4422,12 @@
     <row r="64" spans="2:6">
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
+      <c r="D64" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" s="6"/>
@@ -2091,57 +4660,617 @@
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
     </row>
-    <row r="113" spans="2:3">
+    <row r="113" spans="2:6">
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
     </row>
-    <row r="114" spans="2:3">
+    <row r="114" spans="2:6">
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
     </row>
-    <row r="115" spans="2:3">
+    <row r="115" spans="2:6">
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
     </row>
-    <row r="116" spans="2:3">
+    <row r="116" spans="2:6">
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
     </row>
-    <row r="117" spans="2:3">
+    <row r="117" spans="2:6">
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
     </row>
-    <row r="118" spans="2:3">
+    <row r="118" spans="2:6">
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
     </row>
-    <row r="119" spans="2:3">
+    <row r="119" spans="2:6">
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
     </row>
-    <row r="120" spans="2:3">
+    <row r="120" spans="2:6">
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
     </row>
-    <row r="121" spans="2:3">
+    <row r="121" spans="2:6">
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
     </row>
-    <row r="122" spans="2:3">
+    <row r="122" spans="2:6">
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
     </row>
-    <row r="123" spans="2:3">
+    <row r="123" spans="2:6">
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
     </row>
+    <row r="125" spans="2:6">
+      <c r="B125" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6">
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+    </row>
+    <row r="127" spans="2:6">
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6">
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+    </row>
+    <row r="129" spans="2:5">
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5">
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" spans="2:5">
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+    </row>
+    <row r="132" spans="2:5">
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+    </row>
+    <row r="133" spans="2:5">
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+    </row>
+    <row r="134" spans="2:5">
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+    </row>
+    <row r="135" spans="2:5">
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+    </row>
+    <row r="136" spans="2:5">
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" spans="2:5">
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+    </row>
+    <row r="138" spans="2:5">
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+    </row>
+    <row r="139" spans="2:5">
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+    </row>
+    <row r="140" spans="2:5">
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+    </row>
+    <row r="141" spans="2:5">
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+    </row>
+    <row r="142" spans="2:5">
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+    </row>
+    <row r="143" spans="2:5">
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="2:5">
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+    </row>
+    <row r="145" spans="2:6">
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+    </row>
+    <row r="146" spans="2:6">
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" spans="2:6">
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" spans="2:6">
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="2:6">
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="2:6">
+      <c r="D150" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F150" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6">
+      <c r="B151" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6">
+      <c r="B152" s="6"/>
+      <c r="D152" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="2:6">
+      <c r="B153" s="6"/>
+    </row>
+    <row r="154" spans="2:6" ht="75">
+      <c r="B154" s="6"/>
+      <c r="D154" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E154" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F154" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6">
+      <c r="B155" s="6"/>
+    </row>
+    <row r="156" spans="2:6">
+      <c r="B156" s="6"/>
+    </row>
+    <row r="157" spans="2:6">
+      <c r="B157" s="6"/>
+    </row>
+    <row r="158" spans="2:6">
+      <c r="B158" s="6"/>
+    </row>
+    <row r="159" spans="2:6">
+      <c r="B159" s="6"/>
+    </row>
+    <row r="160" spans="2:6">
+      <c r="B160" s="6"/>
+    </row>
+    <row r="161" spans="2:6">
+      <c r="B161" s="6"/>
+    </row>
+    <row r="162" spans="2:6">
+      <c r="B162" s="6"/>
+    </row>
+    <row r="163" spans="2:6">
+      <c r="B163" s="6"/>
+    </row>
+    <row r="164" spans="2:6">
+      <c r="B164" s="6"/>
+    </row>
+    <row r="165" spans="2:6">
+      <c r="B165" s="6"/>
+    </row>
+    <row r="166" spans="2:6">
+      <c r="B166" s="6"/>
+    </row>
+    <row r="167" spans="2:6">
+      <c r="B167" s="6"/>
+    </row>
+    <row r="168" spans="2:6">
+      <c r="B168" s="6"/>
+    </row>
+    <row r="169" spans="2:6">
+      <c r="B169" s="6"/>
+    </row>
+    <row r="170" spans="2:6">
+      <c r="B170" s="6"/>
+    </row>
+    <row r="171" spans="2:6">
+      <c r="B171" s="5"/>
+    </row>
+    <row r="172" spans="2:6">
+      <c r="B172" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6">
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+    </row>
+    <row r="174" spans="2:6">
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+    </row>
+    <row r="175" spans="2:6">
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+    </row>
+    <row r="176" spans="2:6">
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E176" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="177" spans="2:6">
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+    </row>
+    <row r="178" spans="2:6">
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+    </row>
+    <row r="179" spans="2:6">
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+    </row>
+    <row r="180" spans="2:6">
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+    </row>
+    <row r="181" spans="2:6">
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+      <c r="E181" s="6"/>
+      <c r="F181" s="6"/>
+    </row>
+    <row r="182" spans="2:6">
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+    </row>
+    <row r="183" spans="2:6">
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+    </row>
+    <row r="184" spans="2:6">
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+    </row>
+    <row r="185" spans="2:6">
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
+    </row>
+    <row r="186" spans="2:6">
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+    </row>
+    <row r="187" spans="2:6">
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
+    </row>
+    <row r="188" spans="2:6">
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
+    </row>
+    <row r="189" spans="2:6">
+      <c r="B189" s="6"/>
+      <c r="C189" s="6"/>
+    </row>
+    <row r="190" spans="2:6">
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" spans="2:6">
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+    </row>
+    <row r="192" spans="2:6">
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
+    </row>
+    <row r="193" spans="2:7">
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+    </row>
+    <row r="194" spans="2:7">
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+    </row>
+    <row r="195" spans="2:7">
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+    </row>
+    <row r="197" spans="2:7">
+      <c r="B197" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" ht="45">
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F198" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G198" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7">
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
+    </row>
+    <row r="200" spans="2:7">
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
+    </row>
+    <row r="201" spans="2:7">
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+    </row>
+    <row r="202" spans="2:7">
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
+    </row>
+    <row r="203" spans="2:7">
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
+      <c r="D203" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E203" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7">
+      <c r="B204" s="6"/>
+      <c r="C204" s="6"/>
+    </row>
+    <row r="205" spans="2:7">
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
+    </row>
+    <row r="206" spans="2:7">
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
+    </row>
+    <row r="207" spans="2:7">
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
+    </row>
+    <row r="208" spans="2:7" ht="30">
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E208" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G208" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3">
+      <c r="B209" s="6"/>
+      <c r="C209" s="6"/>
+    </row>
+    <row r="210" spans="2:3">
+      <c r="B210" s="6"/>
+      <c r="C210" s="6"/>
+    </row>
+    <row r="211" spans="2:3">
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
+    </row>
+    <row r="212" spans="2:3">
+      <c r="B212" s="6"/>
+      <c r="C212" s="6"/>
+    </row>
+    <row r="213" spans="2:3">
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
+    </row>
+    <row r="214" spans="2:3">
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+    </row>
+    <row r="215" spans="2:3">
+      <c r="B215" s="6"/>
+      <c r="C215" s="6"/>
+    </row>
+    <row r="216" spans="2:3">
+      <c r="B216" s="6"/>
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" spans="2:3">
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+    </row>
+    <row r="218" spans="2:3">
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
+    </row>
+    <row r="219" spans="2:3">
+      <c r="B219" s="6"/>
+      <c r="C219" s="6"/>
+    </row>
+    <row r="220" spans="2:3">
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+    </row>
+    <row r="221" spans="2:3">
+      <c r="B221" s="6"/>
+      <c r="C221" s="6"/>
+    </row>
+    <row r="224" spans="2:3">
+      <c r="B224" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="225" spans="2:7">
+      <c r="B225" s="6"/>
+    </row>
+    <row r="226" spans="2:7">
+      <c r="B226" s="6"/>
+    </row>
+    <row r="227" spans="2:7">
+      <c r="B227" s="6"/>
+    </row>
+    <row r="228" spans="2:7">
+      <c r="B228" s="6"/>
+    </row>
+    <row r="229" spans="2:7">
+      <c r="B229" s="6"/>
+    </row>
+    <row r="230" spans="2:7">
+      <c r="B230" s="6"/>
+    </row>
+    <row r="231" spans="2:7" ht="30">
+      <c r="B231" s="6"/>
+      <c r="D231" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E231" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F231" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G231" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="232" spans="2:7">
+      <c r="B232" s="6"/>
+    </row>
+    <row r="233" spans="2:7">
+      <c r="B233" s="6"/>
+    </row>
+    <row r="234" spans="2:7">
+      <c r="B234" s="6"/>
+    </row>
+    <row r="235" spans="2:7">
+      <c r="B235" s="6"/>
+    </row>
+    <row r="236" spans="2:7">
+      <c r="B236" s="6"/>
+    </row>
+    <row r="237" spans="2:7">
+      <c r="B237" s="6"/>
+    </row>
+    <row r="238" spans="2:7">
+      <c r="B238" s="6"/>
+    </row>
+    <row r="239" spans="2:7">
+      <c r="B239" s="6"/>
+    </row>
+    <row r="240" spans="2:7">
+      <c r="B240" s="6"/>
+    </row>
+    <row r="241" spans="2:2">
+      <c r="B241" s="6"/>
+    </row>
+    <row r="242" spans="2:2">
+      <c r="B242" s="6"/>
+    </row>
+    <row r="243" spans="2:2">
+      <c r="B243" s="6"/>
+    </row>
+    <row r="244" spans="2:2">
+      <c r="B244" s="6"/>
+    </row>
+    <row r="245" spans="2:2">
+      <c r="B245" s="6"/>
+    </row>
+    <row r="246" spans="2:2">
+      <c r="B246" s="6"/>
+    </row>
+    <row r="247" spans="2:2">
+      <c r="B247" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C4:C29"/>
-    <mergeCell ref="B4:B29"/>
-    <mergeCell ref="B30:B54"/>
-    <mergeCell ref="D4:D29"/>
-    <mergeCell ref="C30:C54"/>
+  <mergeCells count="24">
+    <mergeCell ref="B224:B247"/>
+    <mergeCell ref="D176:D181"/>
+    <mergeCell ref="E176:E181"/>
+    <mergeCell ref="F176:F181"/>
+    <mergeCell ref="B197:B221"/>
+    <mergeCell ref="C197:C221"/>
+    <mergeCell ref="B125:B149"/>
+    <mergeCell ref="C125:C149"/>
+    <mergeCell ref="B151:B170"/>
+    <mergeCell ref="B172:B195"/>
+    <mergeCell ref="C172:C195"/>
     <mergeCell ref="B56:B77"/>
     <mergeCell ref="C56:C77"/>
     <mergeCell ref="G32:G34"/>
@@ -2150,6 +5279,11 @@
     <mergeCell ref="C79:C99"/>
     <mergeCell ref="F79:F81"/>
     <mergeCell ref="C100:C123"/>
+    <mergeCell ref="C4:C29"/>
+    <mergeCell ref="B4:B29"/>
+    <mergeCell ref="B30:B54"/>
+    <mergeCell ref="D4:D29"/>
+    <mergeCell ref="C30:C54"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2161,4 +5295,502 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:R50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.5" style="8" customWidth="1"/>
+    <col min="2" max="18" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:13">
+      <c r="A3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="7"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="K10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="7"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="7"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="7"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="7"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="7"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="7"/>
+      <c r="J22" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="7"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="7"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="O25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="7"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="7"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="7"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="G33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B41:E50"/>
+    <mergeCell ref="O25:Q29"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="E8:F12"/>
+    <mergeCell ref="K10:M14"/>
+    <mergeCell ref="A17:A31"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="G33:I35"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:S43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" style="10" customWidth="1"/>
+    <col min="2" max="19" width="10.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:16">
+      <c r="A4" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="9"/>
+      <c r="O5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+    </row>
+    <row r="20" spans="4:18">
+      <c r="M20" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="4:18">
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="4:18">
+      <c r="D22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="4:18">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="4:18">
+      <c r="Q24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="R24" s="9"/>
+    </row>
+    <row r="25" spans="4:18">
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+    </row>
+    <row r="26" spans="4:18">
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="4:18">
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+    </row>
+    <row r="28" spans="4:18">
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+    </row>
+    <row r="29" spans="4:18">
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+    </row>
+    <row r="30" spans="4:18">
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+    </row>
+    <row r="31" spans="4:18">
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+    </row>
+    <row r="32" spans="4:18">
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="H33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="G40" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="H33:K36"/>
+    <mergeCell ref="Q24:R33"/>
+    <mergeCell ref="A34:B40"/>
+    <mergeCell ref="G40:H43"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="O5:P16"/>
+    <mergeCell ref="M20:N21"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>